<commit_message>
log4j2 used for logging
</commit_message>
<xml_diff>
--- a/conf/Controller.xlsx
+++ b/conf/Controller.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t>SL No</t>
   </si>
@@ -51,10 +51,10 @@
     <t>REG</t>
   </si>
   <si>
-    <t>REG1</t>
-  </si>
-  <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>sachin</t>
   </si>
 </sst>
 </file>
@@ -372,14 +372,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -416,25 +417,96 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>